<commit_message>
add test for shutdown tags
</commit_message>
<xml_diff>
--- a/Waterfall 3.0 to 3.2.xlsx
+++ b/Waterfall 3.0 to 3.2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2790" yWindow="0" windowWidth="27870" windowHeight="11295" activeTab="3"/>
+    <workbookView xWindow="2790" yWindow="0" windowWidth="27870" windowHeight="11295"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="4" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1883" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1884" uniqueCount="248">
   <si>
     <t>H7</t>
   </si>
@@ -1273,6 +1273,9 @@
   </si>
   <si>
     <t>formulas used</t>
+  </si>
+  <si>
+    <t>Remove Integrity Only</t>
   </si>
 </sst>
 </file>
@@ -1362,7 +1365,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB"/>
-              <a:t>Criticality Changes From Systems Feedback (3.0-&gt;3.1)</a:t>
+              <a:t>Criticality Changes From Systems Feedback (3.0-&gt;3.2), Remove Integrity Only Codes</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1447,6 +1450,12 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="102"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-2.8642447849963833E-2"/>
+                  <c:y val="0"/>
+                </c:manualLayout>
+              </c:layout>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
               <c:showCatName val="0"/>
@@ -1457,6 +1466,27 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{0000000E-3808-4096-996C-A11D2D6651F0}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="103"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="2.4550669585683287E-2"/>
+                  <c:y val="0"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-FA49-4DEC-BDEB-6F854A25B7A0}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -1516,9 +1546,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>After!$A$5:$A$107</c:f>
+              <c:f>After!$A$5:$A$108</c:f>
               <c:strCache>
-                <c:ptCount val="102"/>
+                <c:ptCount val="104"/>
                 <c:pt idx="0">
                   <c:v>00</c:v>
                 </c:pt>
@@ -1824,16 +1854,19 @@
                 </c:pt>
                 <c:pt idx="101">
                   <c:v>N/A</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>Remove Integrity Only</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>After!$M$5:$M$107</c:f>
+              <c:f>After!$M$5:$M$108</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="103"/>
+                <c:ptCount val="104"/>
                 <c:pt idx="0">
                   <c:v>6814</c:v>
                 </c:pt>
@@ -2142,6 +2175,9 @@
                 </c:pt>
                 <c:pt idx="102">
                   <c:v>3273</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>3167</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2196,6 +2232,12 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="102"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-3.5462078290431416E-2"/>
+                  <c:y val="0"/>
+                </c:manualLayout>
+              </c:layout>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
               <c:showCatName val="0"/>
@@ -2206,6 +2248,21 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{0000000D-3808-4096-996C-A11D2D6651F0}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="103"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-FA49-4DEC-BDEB-6F854A25B7A0}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -2265,9 +2322,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>After!$A$5:$A$107</c:f>
+              <c:f>After!$A$5:$A$108</c:f>
               <c:strCache>
-                <c:ptCount val="102"/>
+                <c:ptCount val="104"/>
                 <c:pt idx="0">
                   <c:v>00</c:v>
                 </c:pt>
@@ -2573,16 +2630,19 @@
                 </c:pt>
                 <c:pt idx="101">
                   <c:v>N/A</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>Remove Integrity Only</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>After!$N$5:$N$107</c:f>
+              <c:f>After!$N$5:$N$108</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="103"/>
+                <c:ptCount val="104"/>
                 <c:pt idx="0">
                   <c:v>24513</c:v>
                 </c:pt>
@@ -2891,6 +2951,9 @@
                 </c:pt>
                 <c:pt idx="102">
                   <c:v>12561</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>8793</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2945,6 +3008,12 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="102"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-3.8189930466618546E-2"/>
+                  <c:y val="0"/>
+                </c:manualLayout>
+              </c:layout>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
               <c:showCatName val="0"/>
@@ -2955,6 +3024,21 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000011-3808-4096-996C-A11D2D6651F0}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="103"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-FA49-4DEC-BDEB-6F854A25B7A0}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -3014,9 +3098,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>After!$A$5:$A$107</c:f>
+              <c:f>After!$A$5:$A$108</c:f>
               <c:strCache>
-                <c:ptCount val="102"/>
+                <c:ptCount val="104"/>
                 <c:pt idx="0">
                   <c:v>00</c:v>
                 </c:pt>
@@ -3322,16 +3406,19 @@
                 </c:pt>
                 <c:pt idx="101">
                   <c:v>N/A</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>Remove Integrity Only</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>After!$O$5:$O$107</c:f>
+              <c:f>After!$O$5:$O$108</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="103"/>
+                <c:ptCount val="104"/>
                 <c:pt idx="0">
                   <c:v>6292</c:v>
                 </c:pt>
@@ -3640,6 +3727,9 @@
                 </c:pt>
                 <c:pt idx="102">
                   <c:v>21162</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>12409</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3704,6 +3794,21 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000012-3808-4096-996C-A11D2D6651F0}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="103"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-FA49-4DEC-BDEB-6F854A25B7A0}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -3763,9 +3868,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>After!$A$5:$A$107</c:f>
+              <c:f>After!$A$5:$A$108</c:f>
               <c:strCache>
-                <c:ptCount val="102"/>
+                <c:ptCount val="104"/>
                 <c:pt idx="0">
                   <c:v>00</c:v>
                 </c:pt>
@@ -4071,16 +4176,19 @@
                 </c:pt>
                 <c:pt idx="101">
                   <c:v>N/A</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>Remove Integrity Only</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>After!$P$5:$P$107</c:f>
+              <c:f>After!$P$5:$P$108</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="103"/>
+                <c:ptCount val="104"/>
                 <c:pt idx="0">
                   <c:v>44</c:v>
                 </c:pt>
@@ -4389,6 +4497,9 @@
                 </c:pt>
                 <c:pt idx="102">
                   <c:v>667</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>414</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5322,7 +5433,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Chart3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="107" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="107" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5440,7 +5551,13 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-GB" sz="1100" baseline="0"/>
-            <a:t>After: The Rev 3.1 inputs and the effect on the overall totals after applying each update to the Rev 3.0 starting point.</a:t>
+            <a:t>After: The Rev 3.1 inputs and the effect on the overall totals after applying each update to the Rev 3.0 starting point. </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+            <a:t>Append 3.2 results, excluding Integrity Only tags based on Maint / Integrity Split by Failure Class</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -5504,7 +5621,17 @@
             <a:rPr lang="en-GB"/>
             <a:t>)</a:t>
           </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr lvl="1"/>
           <a:endParaRPr lang="en-GB" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:pPr lvl="0"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+            <a:t>3.2 - Exclude integrity only tags</a:t>
+          </a:r>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -5920,7 +6047,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
@@ -9305,10 +9432,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:P107"/>
+  <dimension ref="A1:P108"/>
   <sheetViews>
-    <sheetView topLeftCell="A75" workbookViewId="0">
-      <selection activeCell="P3" sqref="P3"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="P109" sqref="P109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14545,6 +14672,23 @@
         <v>667</v>
       </c>
     </row>
+    <row r="108" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>247</v>
+      </c>
+      <c r="M108">
+        <v>3167</v>
+      </c>
+      <c r="N108">
+        <v>8793</v>
+      </c>
+      <c r="O108">
+        <v>12409</v>
+      </c>
+      <c r="P108">
+        <v>414</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
apply some default rules for equipment
</commit_message>
<xml_diff>
--- a/Waterfall 3.0 to 3.2.xlsx
+++ b/Waterfall 3.0 to 3.2.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://addenergygroup-my.sharepoint.com/personal/douglas_crooke_addenergy_no/Documents/CriticalityVBA/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Douglas.Crooke\OneDrive - add energy group\CriticalityVBA\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2790" yWindow="0" windowWidth="27870" windowHeight="11295"/>
+    <workbookView xWindow="3720" yWindow="0" windowWidth="27870" windowHeight="11295" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="4" r:id="rId1"/>
@@ -1422,9 +1422,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1">
-                <a:alpha val="70000"/>
-              </a:schemeClr>
+              <a:srgbClr val="FFC000"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -2204,9 +2202,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent2">
-                <a:alpha val="70000"/>
-              </a:schemeClr>
+              <a:srgbClr val="FFFF00"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -2980,9 +2976,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent3">
-                <a:alpha val="70000"/>
-              </a:schemeClr>
+              <a:srgbClr val="92D050"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -3756,7 +3750,8 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent4">
+              <a:schemeClr val="bg1">
+                <a:lumMod val="65000"/>
                 <a:alpha val="70000"/>
               </a:schemeClr>
             </a:solidFill>
@@ -5433,7 +5428,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Chart3"/>
   <sheetViews>
-    <sheetView zoomScale="107" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="107" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -6047,7 +6042,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>

</xml_diff>